<commit_message>
Bid status test cases
</commit_message>
<xml_diff>
--- a/testing/testcases.xlsx
+++ b/testing/testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SECRET-BIOS\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74116ECD-5DF9-4E6F-91DB-34D63D231FD1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B58D972-921A-4C33-8B15-7BAE547FBB39}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{10323AF9-E392-FB40-9A7B-EEF537E5AD9C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{10323AF9-E392-FB40-9A7B-EEF537E5AD9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Iter 1-Manual-Login Bootstrap" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Iter 3-Manual-StartClearRound" sheetId="6" r:id="rId5"/>
     <sheet name="Iter 3-JSON-StartClearRound" sheetId="7" r:id="rId6"/>
     <sheet name="Iter 3-JSON-Dump" sheetId="10" r:id="rId7"/>
+    <sheet name="Iter 3 - JSON - Bid Status" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="380">
   <si>
     <t>S/N</t>
   </si>
@@ -3585,14 +3586,84 @@
    "section": "S1"
 }</t>
   </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>{
+    "status": "success",
+    "vacancy": 2,
+    "min-bid-amount": 13.0,
+    "students": [
+        {
+            "userid": "funny",
+            "amount": 30.0,
+            "balance": 20.0, 
+            "status": "success"
+        },
+        {
+            "userid": "apple",
+            "amount": 12.0,
+            "balance": 38.0, 
+            "status": "success"
+        }
+    ]
+}</t>
+  </si>
+  <si>
+    <t>Validate that admin is able to retrieve a comprehensive bid information given a valid section and a valid course</t>
+  </si>
+  <si>
+    <t>r={
+         "course": "IS100",
+         "section": "S1"
+}</t>
+  </si>
+  <si>
+    <t>r={
+         "course": "IS100",
+         "section": "S99"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [ "invalid section" ]
+}</t>
+  </si>
+  <si>
+    <t>{
+    "status": "error",
+    "message": [ "invalid course" ]
+}</t>
+  </si>
+  <si>
+    <t>Validate that admin is unable to retrieve a comprehensive bid information given a valid section but an invalid course</t>
+  </si>
+  <si>
+    <t>r={
+         "course": "IS110",
+         "section": "S1"
+}</t>
+  </si>
+  <si>
+    <t>Validate that admin is unable to retrieve a comprehensive bid information given a valid course but an invalid section</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3755,20 +3826,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3786,63 +3857,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3850,13 +3930,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3864,47 +3950,32 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3916,10 +3987,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3931,45 +4002,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3978,13 +4049,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5584,8 +5661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC4EA0D-1DD6-41E4-AA15-D72AC1FBD4F7}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6687,7 +6764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698A8EA7-29D0-4D6B-801F-D8D6ACD01CF3}">
   <dimension ref="A1:K272"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -6731,7 +6808,7 @@
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
     </row>
-    <row r="2" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A2" s="62">
         <v>1</v>
       </c>
@@ -6756,7 +6833,7 @@
       <c r="J2" s="26"/>
       <c r="K2" s="26"/>
     </row>
-    <row r="3" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A3" s="62">
         <v>2</v>
       </c>
@@ -6829,7 +6906,7 @@
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
     </row>
-    <row r="6" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="62"/>
       <c r="B6" s="63" t="s">
         <v>142</v>
@@ -6852,7 +6929,7 @@
       <c r="J6" s="26"/>
       <c r="K6" s="26"/>
     </row>
-    <row r="7" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="62">
         <v>4</v>
       </c>
@@ -6877,7 +6954,7 @@
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
     </row>
-    <row r="8" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A8" s="62">
         <v>5</v>
       </c>
@@ -6902,7 +6979,7 @@
       <c r="J8" s="26"/>
       <c r="K8" s="26"/>
     </row>
-    <row r="9" spans="1:11" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A9" s="62">
         <v>6</v>
       </c>
@@ -6952,7 +7029,7 @@
       <c r="J10" s="26"/>
       <c r="K10" s="26"/>
     </row>
-    <row r="11" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A11" s="62">
         <v>8</v>
       </c>
@@ -7231,7 +7308,7 @@
       <c r="J21" s="26"/>
       <c r="K21" s="26"/>
     </row>
-    <row r="22" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A22" s="66"/>
       <c r="B22" s="63" t="s">
         <v>307</v>
@@ -7254,7 +7331,7 @@
       <c r="J22" s="26"/>
       <c r="K22" s="26"/>
     </row>
-    <row r="23" spans="1:11" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="144" x14ac:dyDescent="0.3">
       <c r="A23" s="66"/>
       <c r="B23" s="63" t="s">
         <v>307</v>
@@ -7300,7 +7377,7 @@
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
     </row>
-    <row r="25" spans="1:11" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A25" s="66"/>
       <c r="B25" s="63" t="s">
         <v>307</v>
@@ -10697,8 +10774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E8E56E5-054A-466B-9C8A-C203A2EB4217}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" zoomScaleNormal="272" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A28" zoomScale="88" zoomScaleNormal="272" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -11410,8 +11487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197501CD-B915-41CB-BCC7-CA396F9ADD2A}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="93" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="93" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12165,4 +12242,82 @@
     <oddHeader>&amp;C&amp;"Calibri"&amp;8 SMU Classification: Restricted&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5528DBCB-4C58-4E9C-9ECB-E21AAC5CDEA1}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="77" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="28.09765625" customWidth="1"/>
+    <col min="3" max="3" width="25.59765625" customWidth="1"/>
+    <col min="4" max="4" width="30.19921875" customWidth="1"/>
+    <col min="5" max="5" width="11.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A2" s="14"/>
+      <c r="B2" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C2" s="82" t="s">
+        <v>373</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>371</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="C4" s="82" t="s">
+        <v>378</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>376</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>